<commit_message>
Pasted result of orthogonal runs in numbers ran.xlsx
</commit_message>
<xml_diff>
--- a/The numbers ran.xlsx
+++ b/The numbers ran.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspe\Documents\GitHub\StoSim\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40922C29-02E5-45DB-869D-D18E25895D4C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28125"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11028" windowHeight="8724" xr2:uid="{1EDBF45D-93BF-4A95-8445-623CFBEAF877}"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -30,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Sample Size</t>
   </si>
@@ -99,16 +96,19 @@
   </si>
   <si>
     <t>(10000, 1.51015365238709, 0.0074817861089948451)</t>
+  </si>
+  <si>
+    <t>[1.6, 0.0, 1.6, 1.6, 1.6, 1.6, 0.0, 1.6, 1.6, 3.2, 1.6, 1.6, 1.6, 1.6, 3.2, 1.6, 3.2, 1.6, 1.6, 1.6, 1.6, 1.6, 1.6, 3.2, 1.6, 0.0, 1.6, 0.0, 0.0, 0.0, 0.0, 0.0, 1.6, 0.0, 3.2, 0.0, 0.0, 1.6, 1.6, 0.0, 1.92, 2.08, 1.28, 1.6, 1.28, 1.76, 0.8, 1.28, 1.6, 1.44, 1.28, 1.76, 1.76, 1.6, 1.6, 1.76, 1.44, 1.44, 1.92, 1.92, 1.44, 1.6, 1.44, 1.6, 1.6, 1.76, 1.12, 1.44, 1.76, 1.76, 1.44, 1.28, 1.28, 1.44, 1.44, 1.28, 1.28, 1.76, 1.28, 1.92, 1.6, 1.376, 1.376, 1.296, 1.36, 1.536, 1.504, 1.488, 1.408, 1.536, 1.504, 1.376, 1.696, 1.488, 1.36, 1.424, 1.472, 1.568, 1.424, 1.664, 1.44, 1.552, 1.68, 1.664, 1.664, 1.408, 1.712, 1.408, 1.504, 1.552, 1.376, 1.408, 1.504, 1.568, 1.632, 1.696, 1.488, 1.68, 1.536, 1.696, 1.4832, 1.5072, 1.4304, 1.5264, 1.4688, 1.5072, 1.4288, 1.5872, 1.5472, 1.5184, 1.5552, 1.5232, 1.4944, 1.576, 1.5088, 1.528, 1.4976, 1.528, 1.5664, 1.536, 1.5296, 1.5248, 1.4944, 1.5136, 1.488, 1.5184, 1.4976, 1.4608, 1.4768, 1.5072, 1.4864, 1.4416, 1.52, 1.4528, 1.5488, 1.5008, 1.4992, 1.5152, 1.4976, 1.5424, 1.51472, 1.50576, 1.51712, 1.50144, 1.52208, 1.5224, 1.5152, 1.51408, 1.508, 1.51568, 1.4976, 1.5168, 1.52, 1.50816, 1.50464, 1.50912, 1.51712, 1.5096, 1.51808, 1.50304, 1.50576, 1.52064, 1.51952, 1.50672, 1.51472, 1.51712, 1.51456, 1.5176, 1.5112, 1.50544, 1.50672, 1.49888, 1.516, 1.50384, 1.5128, 1.52256, 1.51824, 1.50352, 1.5176, 1.51072, 1.50216, 1.511408, 1.514816, 1.505872, 1.506576, 1.506704, 1.512704, 1.506656, 1.50896, 1.506368, 1.517216, 1.51352, 1.508752, 1.511024, 1.514192, 1.508496, 1.508736, 1.514144, 1.51424, 1.50976, 1.508528, 1.509232, 1.516032, 1.511648, 1.509264, 1.511648, 1.505104, 1.515216, 1.503776, 1.511632, 1.513872, 1.511584, 1.514064, 1.506576, 1.510976, 1.513488, 1.516256, 1.513696, 1.511696, 1.506576]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="#,##0.000"/>
-    <numFmt numFmtId="176" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -150,9 +150,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -213,7 +213,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -265,7 +265,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -459,29 +459,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B453555-41DD-440F-935D-675416B31403}">
-  <dimension ref="A1:G23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -489,12 +489,12 @@
         <v>1.50659177</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -511,7 +511,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>10</v>
       </c>
@@ -528,7 +528,7 @@
         <v>1.3763720427199999</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>100</v>
       </c>
@@ -548,7 +548,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>1000</v>
       </c>
@@ -568,7 +568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>10000</v>
       </c>
@@ -588,7 +588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>100000</v>
       </c>
@@ -608,7 +608,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>1000000</v>
       </c>
@@ -628,15 +628,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>10</v>
       </c>
@@ -656,7 +656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>100</v>
       </c>
@@ -676,7 +676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>1000</v>
       </c>
@@ -696,7 +696,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>10000</v>
       </c>
@@ -716,7 +716,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>100000</v>
       </c>
@@ -736,7 +736,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>1000000</v>
       </c>
@@ -750,12 +750,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>1000</v>
       </c>
@@ -775,7 +775,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>10000</v>
       </c>
@@ -795,7 +795,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>100000</v>
       </c>
@@ -815,8 +815,18 @@
         <v>19</v>
       </c>
     </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added means and stds of orthogonal sampling to xlsx
</commit_message>
<xml_diff>
--- a/The numbers ran.xlsx
+++ b/The numbers ran.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Sample Size</t>
   </si>
@@ -98,7 +98,13 @@
     <t>(10000, 1.51015365238709, 0.0074817861089948451)</t>
   </si>
   <si>
-    <t>[1.6, 0.0, 1.6, 1.6, 1.6, 1.6, 0.0, 1.6, 1.6, 3.2, 1.6, 1.6, 1.6, 1.6, 3.2, 1.6, 3.2, 1.6, 1.6, 1.6, 1.6, 1.6, 1.6, 3.2, 1.6, 0.0, 1.6, 0.0, 0.0, 0.0, 0.0, 0.0, 1.6, 0.0, 3.2, 0.0, 0.0, 1.6, 1.6, 0.0, 1.92, 2.08, 1.28, 1.6, 1.28, 1.76, 0.8, 1.28, 1.6, 1.44, 1.28, 1.76, 1.76, 1.6, 1.6, 1.76, 1.44, 1.44, 1.92, 1.92, 1.44, 1.6, 1.44, 1.6, 1.6, 1.76, 1.12, 1.44, 1.76, 1.76, 1.44, 1.28, 1.28, 1.44, 1.44, 1.28, 1.28, 1.76, 1.28, 1.92, 1.6, 1.376, 1.376, 1.296, 1.36, 1.536, 1.504, 1.488, 1.408, 1.536, 1.504, 1.376, 1.696, 1.488, 1.36, 1.424, 1.472, 1.568, 1.424, 1.664, 1.44, 1.552, 1.68, 1.664, 1.664, 1.408, 1.712, 1.408, 1.504, 1.552, 1.376, 1.408, 1.504, 1.568, 1.632, 1.696, 1.488, 1.68, 1.536, 1.696, 1.4832, 1.5072, 1.4304, 1.5264, 1.4688, 1.5072, 1.4288, 1.5872, 1.5472, 1.5184, 1.5552, 1.5232, 1.4944, 1.576, 1.5088, 1.528, 1.4976, 1.528, 1.5664, 1.536, 1.5296, 1.5248, 1.4944, 1.5136, 1.488, 1.5184, 1.4976, 1.4608, 1.4768, 1.5072, 1.4864, 1.4416, 1.52, 1.4528, 1.5488, 1.5008, 1.4992, 1.5152, 1.4976, 1.5424, 1.51472, 1.50576, 1.51712, 1.50144, 1.52208, 1.5224, 1.5152, 1.51408, 1.508, 1.51568, 1.4976, 1.5168, 1.52, 1.50816, 1.50464, 1.50912, 1.51712, 1.5096, 1.51808, 1.50304, 1.50576, 1.52064, 1.51952, 1.50672, 1.51472, 1.51712, 1.51456, 1.5176, 1.5112, 1.50544, 1.50672, 1.49888, 1.516, 1.50384, 1.5128, 1.52256, 1.51824, 1.50352, 1.5176, 1.51072, 1.50216, 1.511408, 1.514816, 1.505872, 1.506576, 1.506704, 1.512704, 1.506656, 1.50896, 1.506368, 1.517216, 1.51352, 1.508752, 1.511024, 1.514192, 1.508496, 1.508736, 1.514144, 1.51424, 1.50976, 1.508528, 1.509232, 1.516032, 1.511648, 1.509264, 1.511648, 1.505104, 1.515216, 1.503776, 1.511632, 1.513872, 1.511584, 1.514064, 1.506576, 1.510976, 1.513488, 1.516256, 1.513696, 1.511696, 1.506576]</t>
+    <t>Orthogonal Sampling</t>
+  </si>
+  <si>
+    <t>[1.32, 1.536, 1.5155999999999998, 1.50836, 1.5121200000000001, 1.5105792]</t>
+  </si>
+  <si>
+    <t>[1.0047885349664378, 0.25996922894835073, 0.11559861590866907, 0.035726942214524875, 0.006726829862572712, 0.003651293600903659]</t>
   </si>
 </sst>
 </file>
@@ -110,7 +116,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
     <numFmt numFmtId="166" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +128,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,8 +166,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -154,7 +186,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -459,7 +501,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -467,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -752,12 +794,12 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="B21">
         <v>1000</v>
@@ -766,18 +808,18 @@
         <v>40</v>
       </c>
       <c r="D21">
-        <v>1.48713518375</v>
+        <v>1.32</v>
       </c>
       <c r="E21">
-        <v>3.1764300000000002E-2</v>
+        <v>1.0047885349664301</v>
       </c>
       <c r="G21" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22">
-        <v>10000</v>
+        <v>100</v>
       </c>
       <c r="B22">
         <v>1000</v>
@@ -786,38 +828,146 @@
         <v>40</v>
       </c>
       <c r="D22">
-        <v>1.5101536523000001</v>
+        <v>1.536</v>
       </c>
       <c r="E22">
-        <v>7.4817859999999998E-3</v>
+        <v>0.25996922894835001</v>
       </c>
       <c r="G22" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23">
+        <v>1000</v>
+      </c>
+      <c r="B23">
+        <v>1000</v>
+      </c>
+      <c r="C23">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>1.5155999999999901</v>
+      </c>
+      <c r="E23">
+        <v>0.115598615908669</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>10000</v>
+      </c>
+      <c r="B24">
+        <v>1000</v>
+      </c>
+      <c r="C24">
+        <v>40</v>
+      </c>
+      <c r="D24">
+        <v>1.5083599999999999</v>
+      </c>
+      <c r="E24">
+        <v>3.5726942214524798E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
         <v>100000</v>
       </c>
-      <c r="B23">
-        <v>1000</v>
-      </c>
-      <c r="C23">
-        <v>40</v>
-      </c>
-      <c r="D23" s="4">
+      <c r="B25">
+        <v>1000</v>
+      </c>
+      <c r="C25">
+        <v>40</v>
+      </c>
+      <c r="D25">
+        <v>1.5121199999999999</v>
+      </c>
+      <c r="E25">
+        <v>6.7268298625727096E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>1000000</v>
+      </c>
+      <c r="B26">
+        <v>1000</v>
+      </c>
+      <c r="C26">
+        <v>40</v>
+      </c>
+      <c r="D26">
+        <v>1.5105792</v>
+      </c>
+      <c r="E26">
+        <v>3.6512936009036501E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>1000</v>
+      </c>
+      <c r="B29">
+        <v>1000</v>
+      </c>
+      <c r="C29">
+        <v>40</v>
+      </c>
+      <c r="D29">
+        <v>1.48713518375</v>
+      </c>
+      <c r="E29">
+        <v>3.1764300000000002E-2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>10000</v>
+      </c>
+      <c r="B30">
+        <v>1000</v>
+      </c>
+      <c r="C30">
+        <v>40</v>
+      </c>
+      <c r="D30">
+        <v>1.5101536523000001</v>
+      </c>
+      <c r="E30">
+        <v>7.4817859999999998E-3</v>
+      </c>
+      <c r="G30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>100000</v>
+      </c>
+      <c r="B31">
+        <v>1000</v>
+      </c>
+      <c r="C31">
+        <v>40</v>
+      </c>
+      <c r="D31" s="4">
         <v>1.5063534000000001</v>
       </c>
-      <c r="E23">
+      <c r="E31">
         <v>2.3640000000000002E-3</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G31" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added orthogonal sampling to plotErrorbar
</commit_message>
<xml_diff>
--- a/The numbers ran.xlsx
+++ b/The numbers ran.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Sample Size</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>[1.0047885349664378, 0.25996922894835073, 0.11559861590866907, 0.035726942214524875, 0.006726829862572712, 0.003651293600903659]</t>
+  </si>
+  <si>
+    <t>means</t>
+  </si>
+  <si>
+    <t>stds</t>
   </si>
 </sst>
 </file>
@@ -509,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -758,7 +764,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>100000</v>
       </c>
@@ -778,7 +784,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>1000000</v>
       </c>
@@ -792,12 +798,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>10</v>
       </c>
@@ -814,10 +820,13 @@
         <v>1.0047885349664301</v>
       </c>
       <c r="G21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>100</v>
       </c>
@@ -834,10 +843,13 @@
         <v>0.25996922894835001</v>
       </c>
       <c r="G22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>1000</v>
       </c>
@@ -854,7 +866,7 @@
         <v>0.115598615908669</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>10000</v>
       </c>
@@ -871,7 +883,7 @@
         <v>3.5726942214524798E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>100000</v>
       </c>
@@ -888,7 +900,7 @@
         <v>6.7268298625727096E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>1000000</v>
       </c>
@@ -905,12 +917,12 @@
         <v>3.6512936009036501E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:8">
       <c r="A28" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>1000</v>
       </c>
@@ -930,7 +942,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>10000</v>
       </c>
@@ -950,7 +962,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>100000</v>
       </c>

</xml_diff>

<commit_message>
Created a first orthogonal sampling figure
</commit_message>
<xml_diff>
--- a/The numbers ran.xlsx
+++ b/The numbers ran.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Sample Size</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>stds</t>
+  </si>
+  <si>
+    <t>We assume the truw area of the mandelbrot set is the middle of the upper and lower bound of the estimation by Kerry Mitchell</t>
+  </si>
+  <si>
+    <t>Absolute(Mean - true area) -&gt; precision</t>
+  </si>
+  <si>
+    <t>precision * sample size</t>
   </si>
 </sst>
 </file>
@@ -172,8 +181,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -192,17 +207,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -515,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -527,9 +548,10 @@
     <col min="2" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -537,12 +559,12 @@
         <v>1.50659177</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -558,8 +580,20 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4">
+        <v>1.50648</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>10</v>
       </c>
@@ -575,8 +609,16 @@
       <c r="E5" s="1">
         <v>1.3763720427199999</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="F5" s="1">
+        <f>ABS(D5 - $I$4)</f>
+        <v>6.6480000000000095E-2</v>
+      </c>
+      <c r="G5" s="1">
+        <f>F5 * A5</f>
+        <v>0.66480000000000095</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>100</v>
       </c>
@@ -592,11 +634,19 @@
       <c r="E6" s="1">
         <v>0.58191408</v>
       </c>
-      <c r="G6" t="s">
+      <c r="F6" s="1">
+        <f>ABS(D6 - $I$4)</f>
+        <v>0.11752000000000007</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" ref="G6:G31" si="0">F6 * A6</f>
+        <v>11.752000000000006</v>
+      </c>
+      <c r="I6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>1000</v>
       </c>
@@ -612,11 +662,19 @@
       <c r="E7" s="1">
         <v>0.1147763</v>
       </c>
-      <c r="G7" t="s">
+      <c r="F7" s="1">
+        <f>ABS(D7 - $I$4)</f>
+        <v>1.648000000000005E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>16.48000000000005</v>
+      </c>
+      <c r="I7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>10000</v>
       </c>
@@ -632,11 +690,19 @@
       <c r="E8" s="1">
         <v>4.1565832121999997E-2</v>
       </c>
-      <c r="G8" t="s">
+      <c r="F8" s="1">
+        <f>ABS(D8 - $I$4)</f>
+        <v>1.3679999999999914E-2</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>136.79999999999916</v>
+      </c>
+      <c r="I8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>100000</v>
       </c>
@@ -652,11 +718,19 @@
       <c r="E9" s="1">
         <v>1.77965385398E-2</v>
       </c>
-      <c r="G9" t="s">
+      <c r="F9" s="1">
+        <f>ABS(D9 - $I$4)</f>
+        <v>1.9240000000000368E-3</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>192.40000000000367</v>
+      </c>
+      <c r="I9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>1000000</v>
       </c>
@@ -672,19 +746,31 @@
       <c r="E10" s="1">
         <v>4.2900290699999996E-3</v>
       </c>
-      <c r="G10" t="s">
+      <c r="F10" s="1">
+        <f>ABS(D10 - $I$4)</f>
+        <v>1.9240000000000368E-3</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>1924.0000000000368</v>
+      </c>
+      <c r="I10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:10">
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>10</v>
       </c>
@@ -700,11 +786,19 @@
       <c r="E13">
         <v>1.3290598</v>
       </c>
-      <c r="G13" t="s">
+      <c r="F13" s="1">
+        <f>ABS(D13 - $I$4)</f>
+        <v>0.25351999999999997</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5351999999999997</v>
+      </c>
+      <c r="I13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>100</v>
       </c>
@@ -720,11 +814,19 @@
       <c r="E14">
         <v>0.35487465699999998</v>
       </c>
-      <c r="G14" t="s">
+      <c r="F14" s="1">
+        <f>ABS(D14 - $I$4)</f>
+        <v>5.4480000000000084E-2</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4480000000000084</v>
+      </c>
+      <c r="I14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>1000</v>
       </c>
@@ -740,11 +842,19 @@
       <c r="E15">
         <v>9.7780161586999995E-2</v>
       </c>
-      <c r="G15" t="s">
+      <c r="F15" s="1">
+        <f>ABS(D15 - $I$4)</f>
+        <v>3.6719999999999864E-2</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="0"/>
+        <v>36.719999999999864</v>
+      </c>
+      <c r="I15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>10000</v>
       </c>
@@ -760,11 +870,19 @@
       <c r="E16">
         <v>3.3727282724800002E-2</v>
       </c>
-      <c r="G16" t="s">
+      <c r="F16" s="1">
+        <f>ABS(D16 - $I$4)</f>
+        <v>7.1999999999998732E-3</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="0"/>
+        <v>71.999999999998735</v>
+      </c>
+      <c r="I16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>100000</v>
       </c>
@@ -780,11 +898,19 @@
       <c r="E17">
         <v>1.15742327607492E-2</v>
       </c>
-      <c r="G17" t="s">
+      <c r="F17" s="1">
+        <f>ABS(D17 - $I$4)</f>
+        <v>4.2439999999999145E-3</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="0"/>
+        <v>424.39999999999145</v>
+      </c>
+      <c r="I17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>1000000</v>
       </c>
@@ -794,16 +920,36 @@
       <c r="C18">
         <v>40</v>
       </c>
-      <c r="G18" t="s">
+      <c r="D18">
+        <v>1.5105147999999899</v>
+      </c>
+      <c r="E18">
+        <v>3.2913732331657499E-3</v>
+      </c>
+      <c r="F18" s="1">
+        <f>ABS(D18 - $I$4)</f>
+        <v>4.034799999989902E-3</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="0"/>
+        <v>4034.7999999899021</v>
+      </c>
+      <c r="I18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="19" spans="1:10">
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>10</v>
       </c>
@@ -819,14 +965,22 @@
       <c r="E21">
         <v>1.0047885349664301</v>
       </c>
-      <c r="G21" t="s">
+      <c r="F21" s="1">
+        <f>ABS(D21 - $I$4)</f>
+        <v>0.18647999999999998</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="0"/>
+        <v>1.8647999999999998</v>
+      </c>
+      <c r="I21" t="s">
         <v>26</v>
       </c>
-      <c r="H21" t="s">
+      <c r="J21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>100</v>
       </c>
@@ -842,14 +996,22 @@
       <c r="E22">
         <v>0.25996922894835001</v>
       </c>
-      <c r="G22" t="s">
+      <c r="F22" s="1">
+        <f>ABS(D22 - $I$4)</f>
+        <v>2.9519999999999991E-2</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="0"/>
+        <v>2.9519999999999991</v>
+      </c>
+      <c r="I22" t="s">
         <v>27</v>
       </c>
-      <c r="H22" t="s">
+      <c r="J22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>1000</v>
       </c>
@@ -865,8 +1027,16 @@
       <c r="E23">
         <v>0.115598615908669</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="F23" s="1">
+        <f>ABS(D23 - $I$4)</f>
+        <v>9.119999999990025E-3</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="0"/>
+        <v>9.119999999990025</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>10000</v>
       </c>
@@ -882,8 +1052,16 @@
       <c r="E24">
         <v>3.5726942214524798E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="F24" s="1">
+        <f>ABS(D24 - $I$4)</f>
+        <v>1.8799999999998818E-3</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="0"/>
+        <v>18.799999999998818</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>100000</v>
       </c>
@@ -899,8 +1077,16 @@
       <c r="E25">
         <v>6.7268298625727096E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="F25" s="1">
+        <f>ABS(D25 - $I$4)</f>
+        <v>5.6399999999998673E-3</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="0"/>
+        <v>563.9999999999867</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>1000000</v>
       </c>
@@ -916,13 +1102,27 @@
       <c r="E26">
         <v>3.6512936009036501E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="F26" s="1">
+        <f>ABS(D26 - $I$4)</f>
+        <v>4.0991999999999695E-3</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="0"/>
+        <v>4099.1999999999698</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>1000</v>
       </c>
@@ -938,11 +1138,19 @@
       <c r="E29">
         <v>3.1764300000000002E-2</v>
       </c>
-      <c r="G29" t="s">
+      <c r="F29" s="1">
+        <f>ABS(D29 - $I$4)</f>
+        <v>1.9344816250000063E-2</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="0"/>
+        <v>19.344816250000065</v>
+      </c>
+      <c r="I29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>10000</v>
       </c>
@@ -958,11 +1166,19 @@
       <c r="E30">
         <v>7.4817859999999998E-3</v>
       </c>
-      <c r="G30" t="s">
+      <c r="F30" s="1">
+        <f>ABS(D30 - $I$4)</f>
+        <v>3.6736523000000521E-3</v>
+      </c>
+      <c r="G30" s="1">
+        <f>F30 * A30</f>
+        <v>36.736523000000517</v>
+      </c>
+      <c r="I30" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>100000</v>
       </c>
@@ -978,7 +1194,15 @@
       <c r="E31">
         <v>2.3640000000000002E-3</v>
       </c>
-      <c r="G31" t="s">
+      <c r="F31" s="1">
+        <f>ABS(D31 - $I$4)</f>
+        <v>1.2659999999997673E-4</v>
+      </c>
+      <c r="G31" s="1">
+        <f>F31 * A31</f>
+        <v>12.659999999997673</v>
+      </c>
+      <c r="I31" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tried some things with the accuracy, but eventually decided the accuracy is well enough represented by the existing graph
</commit_message>
<xml_diff>
--- a/The numbers ran.xlsx
+++ b/The numbers ran.xlsx
@@ -116,10 +116,10 @@
     <t>We assume the truw area of the mandelbrot set is the middle of the upper and lower bound of the estimation by Kerry Mitchell</t>
   </si>
   <si>
-    <t>Absolute(Mean - true area) -&gt; precision</t>
-  </si>
-  <si>
-    <t>precision * sample size</t>
+    <t>accuracy = Absolute(Mean - true area)</t>
+  </si>
+  <si>
+    <t>accuracy * sample size</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>